<commit_message>
update rule & map
</commit_message>
<xml_diff>
--- a/siteMap.xlsx
+++ b/siteMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shmak\Desktop\MYSET\NPN_pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A826E8D-ED7A-479B-830C-9B2D59BB248F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB838A4E-2330-40FD-9D23-134F8E823A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="3825" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15630" yWindow="4845" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="あ" sheetId="3" r:id="rId1"/>
@@ -83,7 +83,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +108,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -121,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -129,6 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -509,13 +516,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="s">

</xml_diff>